<commit_message>
Add inventory verification test and utility
Introduced InventoryTest to verify inventory items using data from Excel. Added getInventoryItems() method to InventoryPage for retrieving item names. Updated test data and report outputs to reflect new test cases and results.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/SauceDemoTestData.xlsx
+++ b/src/test/resources/testdata/SauceDemoTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Project\selenium-saucedemo-automation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D55A0B-A729-4EBA-9552-2EE7913C34AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D484AE0-5262-4BEB-B458-B6543EC863C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C6D7014D-08AE-476C-BFAA-73A02DD08FB1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>username</t>
   </si>
@@ -60,12 +60,6 @@
     <t>wrong_password</t>
   </si>
   <si>
-    <t>invalid_user</t>
-  </si>
-  <si>
-    <t>invalid_password</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
@@ -109,6 +103,24 @@
   </si>
   <si>
     <t>This classic Sauce Labs t-shirt is perfect to wear when cozying up to your keyboard to automate a few tests. Super-soft and comfy ringspun combed cotton.</t>
+  </si>
+  <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>performance_glitch_user</t>
+  </si>
+  <si>
+    <t>error_user</t>
+  </si>
+  <si>
+    <t>visual_user</t>
+  </si>
+  <si>
+    <t>Not in list</t>
+  </si>
+  <si>
+    <t>This is a sample that is not included in the webpage</t>
   </si>
 </sst>
 </file>
@@ -484,13 +496,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DD23D1-68C3-49B2-A891-99EA8CC28B15}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -538,13 +554,54 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -554,10 +611,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786E3B86-3E56-424A-AF74-31C3B861D12A}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,79 +624,90 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1">
         <v>29.99</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>9.99</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
         <v>15.99</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>49.99</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>7.99</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>15.99</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor test data handling and improve reporting
Updated test methods to use string parameters for price and success values, improving compatibility with Excel data. Enhanced screenshot attachment and error handling in TestListener. Changed Maven compiler version to 17 and configured Surefire to use testng.xml. Refactored test names for clarity and improved Excel cell parsing. Updated test data and report output to reflect these changes.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/SauceDemoTestData.xlsx
+++ b/src/test/resources/testdata/SauceDemoTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Project\selenium-saucedemo-automation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D484AE0-5262-4BEB-B458-B6543EC863C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A9CEE6-D048-48D4-8D3A-9CBA0DBFED3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C6D7014D-08AE-476C-BFAA-73A02DD08FB1}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C6D7014D-08AE-476C-BFAA-73A02DD08FB1}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>username</t>
   </si>
@@ -115,12 +115,6 @@
   </si>
   <si>
     <t>visual_user</t>
-  </si>
-  <si>
-    <t>Not in list</t>
-  </si>
-  <si>
-    <t>This is a sample that is not included in the webpage</t>
   </si>
 </sst>
 </file>
@@ -496,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DD23D1-68C3-49B2-A891-99EA8CC28B15}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,14 +590,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -611,10 +597,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786E3B86-3E56-424A-AF74-31C3B861D12A}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,17 +685,6 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="1">
-        <v>15.99</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>